<commit_message>
homepage template integration and 200 payment received on safepay guru(release action still required)
</commit_message>
<xml_diff>
--- a/doc/hourly_log_sheet_24092013.xlsx
+++ b/doc/hourly_log_sheet_24092013.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>Rate</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Tasks</t>
   </si>
   <si>
-    <t>Project: elanora.biz</t>
-  </si>
-  <si>
     <t>Pending Amount</t>
   </si>
   <si>
@@ -117,6 +114,24 @@
   </si>
   <si>
     <t>24/09/2013</t>
+  </si>
+  <si>
+    <t>Homepage Template Integration</t>
+  </si>
+  <si>
+    <t>28/09/2013</t>
+  </si>
+  <si>
+    <t>Released</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>29/09/2013</t>
+  </si>
+  <si>
+    <t>Project: myguitarpal</t>
   </si>
 </sst>
 </file>
@@ -502,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -516,7 +531,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1">
       <c r="A1" s="7" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -582,7 +597,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>10</v>
@@ -611,13 +626,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="E6">
         <v>8</v>
@@ -637,13 +652,13 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="E7">
         <v>4</v>
@@ -663,13 +678,13 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8">
         <v>3.5</v>
@@ -689,13 +704,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -711,10 +726,30 @@
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="4"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="4"/>
+      <c r="A10" s="4">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>13</v>
+      </c>
+      <c r="G10">
+        <v>52</v>
+      </c>
+      <c r="H10" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="4"/>
@@ -782,16 +817,16 @@
     </row>
     <row r="22" spans="1:7">
       <c r="D22" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E22">
         <f>SUM(E6:E20)</f>
-        <v>17.5</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="D23" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E23">
         <v>15</v>
@@ -799,7 +834,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="D24" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E24">
         <v>-2.5</v>
@@ -807,16 +842,16 @@
     </row>
     <row r="25" spans="1:7">
       <c r="D25" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G25">
         <f>SUM(G6:G23)</f>
-        <v>227.5</v>
+        <v>279.5</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="D26" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G26">
         <v>195</v>
@@ -824,7 +859,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="D27" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G27">
         <v>-32.5</v>
@@ -844,7 +879,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -949,40 +984,57 @@
         <v>5</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9">
-        <v>300</v>
+        <v>195</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10">
+        <v>200</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="3"/>
@@ -995,7 +1047,7 @@
         <v>8</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>195</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
added canvas and canvas guitar theme from wordpress repositoryi
</commit_message>
<xml_diff>
--- a/doc/hourly_log_sheet_24092013.xlsx
+++ b/doc/hourly_log_sheet_24092013.xlsx
@@ -518,7 +518,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:N4"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -739,13 +739,13 @@
         <v>34</v>
       </c>
       <c r="E10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F10">
         <v>13</v>
       </c>
       <c r="G10">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="H10" t="s">
         <v>7</v>
@@ -821,7 +821,7 @@
       </c>
       <c r="E22">
         <f>SUM(E6:E20)</f>
-        <v>21.5</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -846,7 +846,7 @@
       </c>
       <c r="G25">
         <f>SUM(G6:G23)</f>
-        <v>279.5</v>
+        <v>292.5</v>
       </c>
     </row>
     <row r="26" spans="1:7">

</xml_diff>

<commit_message>
homepage header and middle content arrow design changes suggested by Mylesi
</commit_message>
<xml_diff>
--- a/doc/hourly_log_sheet_24092013.xlsx
+++ b/doc/hourly_log_sheet_24092013.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
   <si>
     <t>Rate</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>Project: myguitarpal</t>
+  </si>
+  <si>
+    <t>Homepage deisgn changes in header and middle content arrow and integration</t>
+  </si>
+  <si>
+    <t>30/09/2013</t>
   </si>
 </sst>
 </file>
@@ -518,7 +524,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -751,11 +757,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="4"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="4"/>
+    <row r="11" spans="1:14" ht="30">
+      <c r="A11" s="4">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>13</v>
+      </c>
+      <c r="G11">
+        <v>39</v>
+      </c>
+      <c r="H11" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="4"/>
@@ -821,7 +847,7 @@
       </c>
       <c r="E22">
         <f>SUM(E6:E20)</f>
-        <v>22.5</v>
+        <v>25.5</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -846,7 +872,7 @@
       </c>
       <c r="G25">
         <f>SUM(G6:G23)</f>
-        <v>292.5</v>
+        <v>331.5</v>
       </c>
     </row>
     <row r="26" spans="1:7">

</xml_diff>